<commit_message>
up to ross island 15428
</commit_message>
<xml_diff>
--- a/docs/08262013_nh_to_map.xlsx
+++ b/docs/08262013_nh_to_map.xlsx
@@ -2595,7 +2595,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -2732,15 +2732,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -2854,9 +2850,9 @@
   <dimension ref="1:173"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A158" xSplit="0" ySplit="1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A62" xSplit="0" ySplit="1"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A171" activeCellId="0" pane="bottomLeft" sqref="171:171"/>
+      <selection activeCell="A71" activeCellId="0" pane="bottomLeft" sqref="71:71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7226,80 +7222,65 @@
       <c r="AH70" s="30"/>
       <c r="AI70" s="30"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71" s="35">
-      <c r="A71" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B71" s="34" t="n">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="71" s="15">
+      <c r="A71" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="16" t="n">
         <v>15428</v>
       </c>
-      <c r="C71" s="34" t="n">
+      <c r="C71" s="16" t="n">
         <v>20120378</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="E71" s="34" t="s">
+      <c r="E71" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F71" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G71" s="34" t="s">
+      <c r="F71" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H71" s="34" t="s">
+      <c r="H71" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="I71" s="34" t="s">
+      <c r="I71" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="J71" s="34" t="s">
+      <c r="J71" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="K71" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="L71" s="34" t="s">
+      <c r="K71" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L71" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="M71" s="18" t="n">
+      <c r="M71" s="14" t="n">
         <v>41302.5911455208</v>
       </c>
-      <c r="N71" s="34" t="s">
+      <c r="N71" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="O71" s="34" t="s">
+      <c r="O71" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P71" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q71" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="R71" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="S71" s="18" t="n">
+      <c r="P71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R71" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="S71" s="14" t="n">
         <v>41304.627268287</v>
       </c>
-      <c r="T71" s="34"/>
-      <c r="U71" s="0"/>
-      <c r="V71" s="0"/>
-      <c r="W71" s="0"/>
-      <c r="X71" s="0"/>
-      <c r="Y71" s="0"/>
-      <c r="Z71" s="0"/>
-      <c r="AA71" s="0"/>
-      <c r="AB71" s="0"/>
-      <c r="AC71" s="0"/>
-      <c r="AD71" s="0"/>
-      <c r="AE71" s="0"/>
-      <c r="AF71" s="0"/>
-      <c r="AG71" s="0"/>
-      <c r="AH71" s="0"/>
-      <c r="AI71" s="0"/>
+      <c r="T71" s="16"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="72" s="33">
       <c r="A72" s="26" t="s">
@@ -8049,7 +8030,7 @@
       <c r="J84" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K84" s="36" t="n">
+      <c r="K84" s="34" t="n">
         <v>41592</v>
       </c>
       <c r="L84" s="2" t="s">
@@ -11650,7 +11631,7 @@
         <v>41366.5860202199</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95" s="36">
       <c r="A95" s="17" t="s">
         <v>20</v>
       </c>
@@ -11710,7 +11691,7 @@
       </c>
       <c r="T95" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96" s="36">
       <c r="A96" s="17" t="s">
         <v>20</v>
       </c>
@@ -11770,7 +11751,7 @@
       </c>
       <c r="T96" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97" s="36">
       <c r="A97" s="17" t="s">
         <v>20</v>
       </c>
@@ -11830,7 +11811,7 @@
       </c>
       <c r="T97" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98" s="36">
       <c r="A98" s="17" t="s">
         <v>20</v>
       </c>
@@ -11890,7 +11871,7 @@
       </c>
       <c r="T98" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99" s="36">
       <c r="A99" s="17" t="s">
         <v>20</v>
       </c>
@@ -11950,7 +11931,7 @@
       </c>
       <c r="T99" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="100" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="100" s="36">
       <c r="A100" s="17" t="s">
         <v>20</v>
       </c>
@@ -12010,7 +11991,7 @@
       </c>
       <c r="T100" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="101" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="101" s="36">
       <c r="A101" s="17" t="s">
         <v>20</v>
       </c>
@@ -12070,7 +12051,7 @@
       </c>
       <c r="T101" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="102" s="38">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="102" s="37">
       <c r="A102" s="26" t="s">
         <v>20</v>
       </c>
@@ -12130,7 +12111,7 @@
       </c>
       <c r="T102" s="27"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="103" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="103" s="36">
       <c r="A103" s="17" t="s">
         <v>20</v>
       </c>
@@ -12190,7 +12171,7 @@
       </c>
       <c r="T103" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="104" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="104" s="36">
       <c r="A104" s="17" t="s">
         <v>20</v>
       </c>
@@ -12250,7 +12231,7 @@
       </c>
       <c r="T104" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="105" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="105" s="36">
       <c r="A105" s="17" t="s">
         <v>20</v>
       </c>
@@ -12310,7 +12291,7 @@
       </c>
       <c r="T105" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="106" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="106" s="36">
       <c r="A106" s="17" t="s">
         <v>20</v>
       </c>
@@ -12370,7 +12351,7 @@
       </c>
       <c r="T106" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="107" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="107" s="36">
       <c r="A107" s="17" t="s">
         <v>20</v>
       </c>
@@ -12430,7 +12411,7 @@
       </c>
       <c r="T107" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="108" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="108" s="36">
       <c r="A108" s="17" t="s">
         <v>20</v>
       </c>
@@ -12490,7 +12471,7 @@
       </c>
       <c r="T108" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="109" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="109" s="36">
       <c r="A109" s="17" t="s">
         <v>20</v>
       </c>
@@ -12550,7 +12531,7 @@
       </c>
       <c r="T109" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="110" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="110" s="36">
       <c r="A110" s="17" t="s">
         <v>20</v>
       </c>
@@ -12610,7 +12591,7 @@
       </c>
       <c r="T110" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="111" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="111" s="36">
       <c r="A111" s="17" t="s">
         <v>20</v>
       </c>
@@ -12670,7 +12651,7 @@
       </c>
       <c r="T111" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="112" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="112" s="36">
       <c r="A112" s="17" t="s">
         <v>20</v>
       </c>
@@ -12728,7 +12709,7 @@
       </c>
       <c r="T112" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="113" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="113" s="36">
       <c r="A113" s="17" t="s">
         <v>20</v>
       </c>
@@ -12786,7 +12767,7 @@
       </c>
       <c r="T113" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="114" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="114" s="36">
       <c r="A114" s="17" t="s">
         <v>20</v>
       </c>
@@ -12846,7 +12827,7 @@
       </c>
       <c r="T114" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="115" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="115" s="36">
       <c r="A115" s="17" t="s">
         <v>20</v>
       </c>
@@ -12904,7 +12885,7 @@
       </c>
       <c r="T115" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="116" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="116" s="36">
       <c r="A116" s="17" t="s">
         <v>20</v>
       </c>
@@ -12964,7 +12945,7 @@
       </c>
       <c r="T116" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="117" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="117" s="36">
       <c r="A117" s="17" t="s">
         <v>20</v>
       </c>
@@ -13024,7 +13005,7 @@
       </c>
       <c r="T117" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="118" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="118" s="36">
       <c r="A118" s="17" t="s">
         <v>20</v>
       </c>
@@ -13084,7 +13065,7 @@
       </c>
       <c r="T118" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="119" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="119" s="36">
       <c r="A119" s="17" t="s">
         <v>20</v>
       </c>
@@ -13144,7 +13125,7 @@
       </c>
       <c r="T119" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="120" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="120" s="36">
       <c r="A120" s="17" t="s">
         <v>20</v>
       </c>
@@ -13204,7 +13185,7 @@
       </c>
       <c r="T120" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="121" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="121" s="36">
       <c r="A121" s="17" t="s">
         <v>20</v>
       </c>
@@ -13264,7 +13245,7 @@
       </c>
       <c r="T121" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="122" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="122" s="36">
       <c r="A122" s="17" t="s">
         <v>20</v>
       </c>
@@ -13324,7 +13305,7 @@
       </c>
       <c r="T122" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="123" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="123" s="36">
       <c r="A123" s="17" t="s">
         <v>20</v>
       </c>
@@ -13384,7 +13365,7 @@
       </c>
       <c r="T123" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="124" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="124" s="36">
       <c r="A124" s="17" t="s">
         <v>20</v>
       </c>
@@ -13444,7 +13425,7 @@
       </c>
       <c r="T124" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="125" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="125" s="36">
       <c r="A125" s="17" t="s">
         <v>20</v>
       </c>
@@ -13504,7 +13485,7 @@
       </c>
       <c r="T125" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="126" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="126" s="36">
       <c r="A126" s="17" t="s">
         <v>20</v>
       </c>
@@ -13564,7 +13545,7 @@
       </c>
       <c r="T126" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="127" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="127" s="36">
       <c r="A127" s="17" t="s">
         <v>20</v>
       </c>
@@ -13624,7 +13605,7 @@
       </c>
       <c r="T127" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="128" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="128" s="36">
       <c r="A128" s="17" t="s">
         <v>20</v>
       </c>
@@ -13684,7 +13665,7 @@
       </c>
       <c r="T128" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="129" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="129" s="36">
       <c r="A129" s="17" t="s">
         <v>20</v>
       </c>
@@ -13744,7 +13725,7 @@
       </c>
       <c r="T129" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="130" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="130" s="36">
       <c r="A130" s="17" t="s">
         <v>20</v>
       </c>
@@ -13804,7 +13785,7 @@
       </c>
       <c r="T130" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="131" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="131" s="36">
       <c r="A131" s="17" t="s">
         <v>20</v>
       </c>
@@ -13864,7 +13845,7 @@
       </c>
       <c r="T131" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="132" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="132" s="36">
       <c r="A132" s="17" t="s">
         <v>20</v>
       </c>
@@ -13924,7 +13905,7 @@
       </c>
       <c r="T132" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="133" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="133" s="36">
       <c r="A133" s="17" t="s">
         <v>20</v>
       </c>
@@ -13984,7 +13965,7 @@
       </c>
       <c r="T133" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="134" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="134" s="36">
       <c r="A134" s="17" t="s">
         <v>20</v>
       </c>
@@ -14044,7 +14025,7 @@
       </c>
       <c r="T134" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="135" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="135" s="36">
       <c r="A135" s="17" t="s">
         <v>20</v>
       </c>
@@ -14104,7 +14085,7 @@
       </c>
       <c r="T135" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="136" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="136" s="36">
       <c r="A136" s="17" t="s">
         <v>20</v>
       </c>
@@ -14162,7 +14143,7 @@
       </c>
       <c r="T136" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="137" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="137" s="36">
       <c r="A137" s="17" t="s">
         <v>20</v>
       </c>
@@ -14220,7 +14201,7 @@
       </c>
       <c r="T137" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="138" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="138" s="36">
       <c r="A138" s="17" t="s">
         <v>20</v>
       </c>
@@ -14280,7 +14261,7 @@
       </c>
       <c r="T138" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="139" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="139" s="36">
       <c r="A139" s="17" t="s">
         <v>20</v>
       </c>
@@ -14338,7 +14319,7 @@
       </c>
       <c r="T139" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="140" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="140" s="36">
       <c r="A140" s="17" t="s">
         <v>20</v>
       </c>
@@ -14398,7 +14379,7 @@
       </c>
       <c r="T140" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="141" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="141" s="36">
       <c r="A141" s="17" t="s">
         <v>20</v>
       </c>
@@ -14458,7 +14439,7 @@
       </c>
       <c r="T141" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="142" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="142" s="36">
       <c r="A142" s="17" t="s">
         <v>20</v>
       </c>
@@ -14518,7 +14499,7 @@
       </c>
       <c r="T142" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="143" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="143" s="36">
       <c r="A143" s="17" t="s">
         <v>20</v>
       </c>
@@ -14578,7 +14559,7 @@
       </c>
       <c r="T143" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="144" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="144" s="36">
       <c r="A144" s="17" t="s">
         <v>20</v>
       </c>
@@ -14638,7 +14619,7 @@
       </c>
       <c r="T144" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="145" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="145" s="36">
       <c r="A145" s="17" t="s">
         <v>20</v>
       </c>
@@ -14696,7 +14677,7 @@
       </c>
       <c r="T145" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="146" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="146" s="36">
       <c r="A146" s="17" t="s">
         <v>20</v>
       </c>
@@ -14754,7 +14735,7 @@
       </c>
       <c r="T146" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="147" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="147" s="36">
       <c r="A147" s="17" t="s">
         <v>20</v>
       </c>
@@ -14812,7 +14793,7 @@
       </c>
       <c r="T147" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="148" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="148" s="36">
       <c r="A148" s="17" t="s">
         <v>20</v>
       </c>
@@ -14872,7 +14853,7 @@
       </c>
       <c r="T148" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="149" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="149" s="36">
       <c r="A149" s="17" t="s">
         <v>20</v>
       </c>
@@ -14932,7 +14913,7 @@
       </c>
       <c r="T149" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="150" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="150" s="36">
       <c r="A150" s="17" t="s">
         <v>20</v>
       </c>
@@ -14992,7 +14973,7 @@
       </c>
       <c r="T150" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="151" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="151" s="36">
       <c r="A151" s="17" t="s">
         <v>20</v>
       </c>
@@ -15050,7 +15031,7 @@
       </c>
       <c r="T151" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="152" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="152" s="36">
       <c r="A152" s="17" t="s">
         <v>20</v>
       </c>
@@ -15110,7 +15091,7 @@
       </c>
       <c r="T152" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="153" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="153" s="36">
       <c r="A153" s="17" t="s">
         <v>20</v>
       </c>
@@ -15170,7 +15151,7 @@
       </c>
       <c r="T153" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="154" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="154" s="36">
       <c r="A154" s="17" t="s">
         <v>20</v>
       </c>
@@ -15230,7 +15211,7 @@
       </c>
       <c r="T154" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="155" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="155" s="36">
       <c r="A155" s="17" t="s">
         <v>20</v>
       </c>
@@ -15290,7 +15271,7 @@
       </c>
       <c r="T155" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="156" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="156" s="36">
       <c r="A156" s="17" t="s">
         <v>20</v>
       </c>
@@ -15350,7 +15331,7 @@
       </c>
       <c r="T156" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="157" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="157" s="36">
       <c r="A157" s="17" t="s">
         <v>20</v>
       </c>
@@ -15410,7 +15391,7 @@
       </c>
       <c r="T157" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="158" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="158" s="36">
       <c r="A158" s="17" t="s">
         <v>20</v>
       </c>
@@ -15470,7 +15451,7 @@
       </c>
       <c r="T158" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="159" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="159" s="36">
       <c r="A159" s="17" t="s">
         <v>20</v>
       </c>
@@ -15530,7 +15511,7 @@
       </c>
       <c r="T159" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="160" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="160" s="36">
       <c r="A160" s="17" t="s">
         <v>20</v>
       </c>
@@ -15588,7 +15569,7 @@
       </c>
       <c r="T160" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="161" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="161" s="36">
       <c r="A161" s="17" t="s">
         <v>20</v>
       </c>
@@ -15648,7 +15629,7 @@
       </c>
       <c r="T161" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="162" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="162" s="36">
       <c r="A162" s="17" t="s">
         <v>20</v>
       </c>
@@ -15706,7 +15687,7 @@
       </c>
       <c r="T162" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="163" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="163" s="36">
       <c r="A163" s="17" t="s">
         <v>20</v>
       </c>
@@ -15766,7 +15747,7 @@
       </c>
       <c r="T163" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="164" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="164" s="36">
       <c r="A164" s="17" t="s">
         <v>20</v>
       </c>
@@ -15824,7 +15805,7 @@
       </c>
       <c r="T164" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="165" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="165" s="36">
       <c r="A165" s="17" t="s">
         <v>20</v>
       </c>
@@ -15884,7 +15865,7 @@
       </c>
       <c r="T165" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="166" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="166" s="36">
       <c r="A166" s="17" t="s">
         <v>20</v>
       </c>
@@ -15942,312 +15923,312 @@
       </c>
       <c r="T166" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="167" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="167" s="36">
       <c r="A167" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B167" s="39" t="n">
+      <c r="B167" s="38" t="n">
         <v>16085</v>
       </c>
-      <c r="C167" s="39" t="n">
+      <c r="C167" s="38" t="n">
         <v>20130021</v>
       </c>
-      <c r="D167" s="39" t="s">
+      <c r="D167" s="38" t="s">
         <v>788</v>
       </c>
-      <c r="E167" s="39" t="s">
+      <c r="E167" s="38" t="s">
         <v>789</v>
       </c>
       <c r="F167" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G167" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H167" s="39" t="s">
+      <c r="G167" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H167" s="38" t="s">
         <v>790</v>
       </c>
-      <c r="I167" s="39" t="s">
+      <c r="I167" s="38" t="s">
         <v>791</v>
       </c>
-      <c r="J167" s="39" t="s">
+      <c r="J167" s="38" t="s">
         <v>152</v>
       </c>
       <c r="K167" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="L167" s="39" t="s">
+      <c r="L167" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="M167" s="40" t="n">
+      <c r="M167" s="39" t="n">
         <v>41449.3498559028</v>
       </c>
-      <c r="N167" s="39" t="s">
+      <c r="N167" s="38" t="s">
         <v>792</v>
       </c>
-      <c r="O167" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P167" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q167" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="R167" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S167" s="40" t="n">
+      <c r="O167" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="P167" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q167" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R167" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S167" s="39" t="n">
         <v>41449.3675326389</v>
       </c>
       <c r="T167" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="168" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="168" s="36">
       <c r="A168" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B168" s="39" t="n">
+      <c r="B168" s="38" t="n">
         <v>16086</v>
       </c>
-      <c r="C168" s="39" t="n">
+      <c r="C168" s="38" t="n">
         <v>20130022</v>
       </c>
-      <c r="D168" s="39" t="s">
+      <c r="D168" s="38" t="s">
         <v>793</v>
       </c>
-      <c r="E168" s="39" t="s">
+      <c r="E168" s="38" t="s">
         <v>766</v>
       </c>
       <c r="F168" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G168" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H168" s="39" t="s">
+      <c r="G168" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H168" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="I168" s="39" t="n">
-        <v>29</v>
-      </c>
-      <c r="J168" s="39" t="s">
+      <c r="I168" s="38" t="n">
+        <v>29</v>
+      </c>
+      <c r="J168" s="38" t="s">
         <v>736</v>
       </c>
       <c r="K168" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="L168" s="39" t="s">
+      <c r="L168" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="M168" s="40" t="n">
+      <c r="M168" s="39" t="n">
         <v>41449.494916169</v>
       </c>
-      <c r="N168" s="39" t="s">
+      <c r="N168" s="38" t="s">
         <v>794</v>
       </c>
-      <c r="O168" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P168" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q168" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="R168" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S168" s="40" t="n">
+      <c r="O168" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="P168" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q168" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R168" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S168" s="39" t="n">
         <v>41449.5007751968</v>
       </c>
       <c r="T168" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="169" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="169" s="36">
       <c r="A169" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B169" s="39" t="n">
+      <c r="B169" s="38" t="n">
         <v>16087</v>
       </c>
-      <c r="C169" s="39" t="n">
+      <c r="C169" s="38" t="n">
         <v>20130023</v>
       </c>
-      <c r="D169" s="39" t="s">
+      <c r="D169" s="38" t="s">
         <v>795</v>
       </c>
-      <c r="E169" s="39" t="s">
+      <c r="E169" s="38" t="s">
         <v>796</v>
       </c>
-      <c r="F169" s="39" t="s">
+      <c r="F169" s="38" t="s">
         <v>797</v>
       </c>
-      <c r="G169" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H169" s="39" t="s">
+      <c r="G169" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H169" s="38" t="s">
         <v>798</v>
       </c>
-      <c r="I169" s="39" t="s">
+      <c r="I169" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="J169" s="39" t="s">
+      <c r="J169" s="38" t="s">
         <v>763</v>
       </c>
       <c r="K169" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="L169" s="39" t="s">
+      <c r="L169" s="38" t="s">
         <v>798</v>
       </c>
-      <c r="M169" s="40" t="n">
+      <c r="M169" s="39" t="n">
         <v>41449.6461498843</v>
       </c>
-      <c r="N169" s="39" t="s">
+      <c r="N169" s="38" t="s">
         <v>799</v>
       </c>
-      <c r="O169" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P169" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q169" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="R169" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S169" s="40" t="n">
+      <c r="O169" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="P169" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q169" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R169" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S169" s="39" t="n">
         <v>41449.685081331</v>
       </c>
       <c r="T169" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="170" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="170" s="36">
       <c r="A170" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B170" s="39" t="n">
+      <c r="B170" s="38" t="n">
         <v>16089</v>
       </c>
-      <c r="C170" s="39" t="n">
+      <c r="C170" s="38" t="n">
         <v>20130024</v>
       </c>
-      <c r="D170" s="39" t="s">
+      <c r="D170" s="38" t="s">
         <v>800</v>
       </c>
-      <c r="E170" s="39" t="s">
+      <c r="E170" s="38" t="s">
         <v>801</v>
       </c>
-      <c r="F170" s="39" t="s">
+      <c r="F170" s="38" t="s">
         <v>802</v>
       </c>
-      <c r="G170" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H170" s="39" t="s">
+      <c r="G170" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H170" s="38" t="s">
         <v>414</v>
       </c>
-      <c r="I170" s="39" t="s">
+      <c r="I170" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="J170" s="39" t="s">
+      <c r="J170" s="38" t="s">
         <v>803</v>
       </c>
       <c r="K170" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="L170" s="39" t="s">
+      <c r="L170" s="38" t="s">
         <v>410</v>
       </c>
-      <c r="M170" s="40" t="n">
+      <c r="M170" s="39" t="n">
         <v>41450.6984287037</v>
       </c>
-      <c r="N170" s="39" t="s">
+      <c r="N170" s="38" t="s">
         <v>804</v>
       </c>
-      <c r="O170" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P170" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q170" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="R170" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S170" s="40" t="n">
+      <c r="O170" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="P170" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q170" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R170" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S170" s="39" t="n">
         <v>41450.715544294</v>
       </c>
-      <c r="T170" s="39"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="171" s="37">
+      <c r="T170" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="171" s="36">
       <c r="A171" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B171" s="39" t="n">
+      <c r="B171" s="38" t="n">
         <v>16091</v>
       </c>
-      <c r="C171" s="39" t="n">
+      <c r="C171" s="38" t="n">
         <v>20130025</v>
       </c>
-      <c r="D171" s="39" t="s">
+      <c r="D171" s="38" t="s">
         <v>805</v>
       </c>
-      <c r="E171" s="39"/>
-      <c r="F171" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="G171" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H171" s="39" t="s">
+      <c r="E171" s="38"/>
+      <c r="F171" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G171" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H171" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="I171" s="39" t="s">
+      <c r="I171" s="38" t="s">
         <v>573</v>
       </c>
-      <c r="J171" s="39" t="n">
+      <c r="J171" s="38" t="n">
         <v>40</v>
       </c>
-      <c r="K171" s="39" t="s">
+      <c r="K171" s="38" t="s">
         <v>806</v>
       </c>
-      <c r="L171" s="39" t="s">
+      <c r="L171" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="M171" s="40" t="n">
+      <c r="M171" s="39" t="n">
         <v>41451.4667568287</v>
       </c>
-      <c r="N171" s="39" t="s">
+      <c r="N171" s="38" t="s">
         <v>807</v>
       </c>
-      <c r="O171" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="P171" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q171" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="R171" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S171" s="40" t="n">
+      <c r="O171" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="P171" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q171" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R171" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S171" s="39" t="n">
         <v>41451.4801988426</v>
       </c>
       <c r="T171" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="172" s="37">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="172" s="36">
       <c r="A172" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B172" s="39" t="n">
+      <c r="B172" s="38" t="n">
         <v>16093</v>
       </c>
-      <c r="C172" s="39" t="n">
+      <c r="C172" s="38" t="n">
         <v>20130029</v>
       </c>
       <c r="D172" s="0" t="s">
@@ -16300,27 +16281,27 @@
       </c>
       <c r="T172" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="173" s="43">
-      <c r="A173" s="41"/>
-      <c r="B173" s="42"/>
-      <c r="C173" s="42"/>
-      <c r="D173" s="42"/>
-      <c r="E173" s="42"/>
-      <c r="F173" s="42"/>
-      <c r="G173" s="42"/>
-      <c r="H173" s="42"/>
-      <c r="I173" s="42"/>
-      <c r="J173" s="42"/>
-      <c r="K173" s="42"/>
-      <c r="L173" s="42"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="173" s="42">
+      <c r="A173" s="40"/>
+      <c r="B173" s="41"/>
+      <c r="C173" s="41"/>
+      <c r="D173" s="41"/>
+      <c r="E173" s="41"/>
+      <c r="F173" s="41"/>
+      <c r="G173" s="41"/>
+      <c r="H173" s="41"/>
+      <c r="I173" s="41"/>
+      <c r="J173" s="41"/>
+      <c r="K173" s="41"/>
+      <c r="L173" s="41"/>
       <c r="M173" s="18"/>
-      <c r="N173" s="42"/>
-      <c r="O173" s="42"/>
-      <c r="P173" s="42"/>
-      <c r="Q173" s="42"/>
-      <c r="R173" s="42"/>
+      <c r="N173" s="41"/>
+      <c r="O173" s="41"/>
+      <c r="P173" s="41"/>
+      <c r="Q173" s="41"/>
+      <c r="R173" s="41"/>
       <c r="S173" s="18"/>
-      <c r="T173" s="42"/>
+      <c r="T173" s="41"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>